<commit_message>
Update with 0MW min in MARKET
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="11_7D95A7C73E3670CDB74D5D1D2BF767C2935C3038" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F66021E-6C8E-4606-87A0-DFB900B467C1}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_C402FF1093F3E73146009848F450FA7E2DC2A1C5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{031FB188-5195-4E74-AAC8-553F8D545AE6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="21" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -162,9 +162,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,25 +214,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -252,1157 +234,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Market</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="ltUpDiag">
-              <a:fgClr>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>PG_MARKET!$B$1:$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>G1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>G2.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>G2.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>G3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>W1.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>W1.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>W2.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>W2.2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>PG_MARKET!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7D27-450A-88D2-4FD2608D2BFF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Curtailed</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="openDmnd">
-              <a:fgClr>
-                <a:schemeClr val="accent6"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>PG_MARKET!$B$1:$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>G1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>G2.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>G2.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>G3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>W1.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>W1.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>W2.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>W2.2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>PG_SECURE!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30.0959</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>46.301400000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>46.301400000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>46.301400000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7D27-450A-88D2-4FD2608D2BFF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Constrained</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>PG_MARKET!$B$1:$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>G1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>G2.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>G2.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>G3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>W1.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>W1.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>W2.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>W2.2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pG!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2.4980018054066019E-14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30.0959</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>46.301400000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>37.801350000000014</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>37.801350000000014</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7D27-450A-88D2-4FD2608D2BFF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="2102019391"/>
-        <c:axId val="2102019871"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2102019391"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2102019871"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2102019871"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="800" b="0"/>
-                  <a:t>Generator</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="800" b="0" baseline="0"/>
-                  <a:t> Power (MW)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB" sz="800" b="0"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2102019391"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr>
-          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4248D362-0D2D-D2EC-B0B3-96547B818B7E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1695,7 +526,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1753,231 +584,231 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
         <v>269.00000000000011</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2">
+        <v>269</v>
+      </c>
+      <c r="D2">
+        <v>117</v>
+      </c>
+      <c r="E2">
+        <v>240</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>152</v>
+      </c>
+      <c r="H2">
+        <v>87.999999999999972</v>
+      </c>
+      <c r="I2">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="J2">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>49.749999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
         <v>269.00000000000011</v>
       </c>
-      <c r="D2" s="4">
+      <c r="C3">
+        <v>269</v>
+      </c>
+      <c r="D3">
         <v>117</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E3">
         <v>240</v>
       </c>
-      <c r="F2" s="4">
-        <v>21</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>152</v>
       </c>
-      <c r="H2" s="4">
-        <v>66.999999999999972</v>
-      </c>
-      <c r="I2" s="4">
-        <v>49.999899999999997</v>
-      </c>
-      <c r="J2" s="4">
-        <v>17.249999999999989</v>
-      </c>
-      <c r="K2" s="4">
-        <v>32.749900000000018</v>
-      </c>
-      <c r="L2" s="4">
-        <v>17.000099999999971</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="H3">
+        <v>87.999999999999972</v>
+      </c>
+      <c r="I3">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="J3">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>49.749999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
         <v>269.00000000000011</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C4">
+        <v>269</v>
+      </c>
+      <c r="D4">
+        <v>117</v>
+      </c>
+      <c r="E4">
+        <v>240</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>152</v>
+      </c>
+      <c r="H4">
+        <v>87.999999999999972</v>
+      </c>
+      <c r="I4">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="J4">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>49.749999999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
         <v>269.00000000000011</v>
       </c>
-      <c r="D3" s="4">
-        <v>117</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="C5">
+        <v>269.00000000000011</v>
+      </c>
+      <c r="D5">
+        <v>137</v>
+      </c>
+      <c r="E5">
         <v>240</v>
       </c>
-      <c r="F3" s="4">
-        <v>21</v>
-      </c>
-      <c r="G3" s="4">
-        <v>152</v>
-      </c>
-      <c r="H3" s="4">
-        <v>66.999999999999972</v>
-      </c>
-      <c r="I3" s="4">
-        <v>49.999899999999997</v>
-      </c>
-      <c r="J3" s="4">
-        <v>17.249999999999989</v>
-      </c>
-      <c r="K3" s="4">
-        <v>32.749900000000018</v>
-      </c>
-      <c r="L3" s="4">
-        <v>17.000099999999971</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>132</v>
+      </c>
+      <c r="H5">
+        <v>108</v>
+      </c>
+      <c r="I5">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="J5">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>69.749999999999986</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
         <v>269.00000000000011</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C6">
         <v>269.00000000000011</v>
       </c>
-      <c r="D4" s="4">
-        <v>117</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="D6">
+        <v>137</v>
+      </c>
+      <c r="E6">
         <v>240</v>
       </c>
-      <c r="F4" s="4">
-        <v>21</v>
-      </c>
-      <c r="G4" s="4">
-        <v>152</v>
-      </c>
-      <c r="H4" s="4">
-        <v>66.999999999999972</v>
-      </c>
-      <c r="I4" s="4">
-        <v>49.999899999999997</v>
-      </c>
-      <c r="J4" s="4">
-        <v>17.249999999999989</v>
-      </c>
-      <c r="K4" s="4">
-        <v>32.749900000000018</v>
-      </c>
-      <c r="L4" s="4">
-        <v>17.000099999999971</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>132</v>
+      </c>
+      <c r="H6">
+        <v>108</v>
+      </c>
+      <c r="I6">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="J6">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>69.749999999999986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
         <v>269.00000000000011</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C7">
         <v>269.00000000000011</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D7">
         <v>137</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E7">
         <v>240</v>
       </c>
-      <c r="F5" s="4">
-        <v>21</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>132</v>
       </c>
-      <c r="H5" s="4">
-        <v>86.999999999999986</v>
-      </c>
-      <c r="I5" s="4">
-        <v>49.999899999999997</v>
-      </c>
-      <c r="J5" s="4">
-        <v>17.249999999999989</v>
-      </c>
-      <c r="K5" s="4">
-        <v>32.749900000000018</v>
-      </c>
-      <c r="L5" s="4">
-        <v>37.000099999999989</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4">
-        <v>269.00000000000011</v>
-      </c>
-      <c r="C6" s="4">
-        <v>269.00000000000011</v>
-      </c>
-      <c r="D6" s="4">
-        <v>137</v>
-      </c>
-      <c r="E6" s="4">
-        <v>240</v>
-      </c>
-      <c r="F6" s="4">
-        <v>21</v>
-      </c>
-      <c r="G6" s="4">
-        <v>132</v>
-      </c>
-      <c r="H6" s="4">
-        <v>86.999999999999986</v>
-      </c>
-      <c r="I6" s="4">
-        <v>49.999899999999997</v>
-      </c>
-      <c r="J6" s="4">
-        <v>17.249999999999989</v>
-      </c>
-      <c r="K6" s="4">
-        <v>32.749900000000018</v>
-      </c>
-      <c r="L6" s="4">
-        <v>37.000099999999989</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4">
-        <v>269.00000000000011</v>
-      </c>
-      <c r="C7" s="4">
-        <v>269.00000000000011</v>
-      </c>
-      <c r="D7" s="4">
-        <v>137</v>
-      </c>
-      <c r="E7" s="4">
-        <v>240</v>
-      </c>
-      <c r="F7" s="4">
-        <v>21</v>
-      </c>
-      <c r="G7" s="4">
-        <v>132</v>
-      </c>
-      <c r="H7" s="4">
-        <v>86.999999999999986</v>
-      </c>
-      <c r="I7" s="4">
-        <v>49.999899999999997</v>
-      </c>
-      <c r="J7" s="4">
-        <v>17.249999999999989</v>
-      </c>
-      <c r="K7" s="4">
-        <v>32.749900000000018</v>
-      </c>
-      <c r="L7" s="4">
-        <v>37.000099999999989</v>
+      <c r="H7">
+        <v>108</v>
+      </c>
+      <c r="I7">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="J7">
+        <v>38.249999999999993</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>69.749999999999986</v>
       </c>
     </row>
   </sheetData>
@@ -2015,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>17.000099999999971</v>
+        <v>49.749999999999993</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2029,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>17.000099999999971</v>
+        <v>49.749999999999993</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2043,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>17.000099999999971</v>
+        <v>49.749999999999993</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -2057,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>37.000099999999989</v>
+        <v>69.749999999999986</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2071,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>37.000099999999989</v>
+        <v>69.749999999999986</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -2085,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>37.000099999999989</v>
+        <v>69.749999999999986</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2234,7 +1065,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2248,7 +1079,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2262,7 +1093,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2345,7 +1176,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>1.0636694938096589</v>
+        <v>1.1806354002520869</v>
       </c>
       <c r="C2">
         <v>0.96142318022952133</v>
@@ -2359,7 +1190,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>1.0636694938096589</v>
+        <v>1.1806354002520869</v>
       </c>
       <c r="C3">
         <v>0.96142318022952133</v>
@@ -2373,7 +1204,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>1.0636694938096589</v>
+        <v>1.1806354002520869</v>
       </c>
       <c r="C4">
         <v>0.96142318022952133</v>
@@ -2387,7 +1218,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>1.1318337028630849</v>
+        <v>1.32677688026713</v>
       </c>
       <c r="C5">
         <v>0.96142318022952133</v>
@@ -2401,7 +1232,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>1.1318337028630849</v>
+        <v>1.32677688026713</v>
       </c>
       <c r="C6">
         <v>0.96142318022952133</v>
@@ -2415,7 +1246,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>1.1318337028630849</v>
+        <v>1.32677688026713</v>
       </c>
       <c r="C7">
         <v>0.96142318022952133</v>
@@ -2453,10 +1284,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.102246313580138</v>
+        <v>0.21921222002256521</v>
       </c>
       <c r="C2">
-        <v>0.102246313580138</v>
+        <v>0.21921222002256521</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2464,10 +1295,10 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0.102246313580138</v>
+        <v>0.21921222002256521</v>
       </c>
       <c r="C3">
-        <v>0.102246313580138</v>
+        <v>0.21921222002256521</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2475,10 +1306,10 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.102246313580138</v>
+        <v>0.21921222002256521</v>
       </c>
       <c r="C4">
-        <v>0.102246313580138</v>
+        <v>0.21921222002256521</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2486,10 +1317,10 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0.1704105226335634</v>
+        <v>0.36535370003760848</v>
       </c>
       <c r="C5">
-        <v>0.1704105226335634</v>
+        <v>0.36535370003760859</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2497,10 +1328,10 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>0.1704105226335634</v>
+        <v>0.36535370003760848</v>
       </c>
       <c r="C6">
-        <v>0.1704105226335634</v>
+        <v>0.36535370003760859</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2508,10 +1339,10 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0.1704105226335634</v>
+        <v>0.36535370003760848</v>
       </c>
       <c r="C7">
-        <v>0.1704105226335634</v>
+        <v>0.36535370003760859</v>
       </c>
     </row>
   </sheetData>
@@ -2633,10 +1464,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>12.838380000000001</v>
+        <v>27.525000000000009</v>
       </c>
       <c r="C2">
-        <v>8.5589199999999988</v>
+        <v>18.350000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2644,10 +1475,10 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>12.838380000000001</v>
+        <v>27.525000000000009</v>
       </c>
       <c r="C3">
-        <v>8.5589199999999988</v>
+        <v>18.350000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2655,10 +1486,10 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>12.838380000000001</v>
+        <v>27.525000000000009</v>
       </c>
       <c r="C4">
-        <v>8.5589199999999988</v>
+        <v>18.350000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2666,7 +1497,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>21.397300000000001</v>
+        <v>45.875</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2677,7 +1508,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>21.397300000000001</v>
+        <v>45.875</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2688,7 +1519,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>21.397300000000001</v>
+        <v>45.875</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2793,9 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2829,177 +1658,177 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2">
+        <v>5.5511151231257827E-15</v>
+      </c>
+      <c r="C2">
         <v>50</v>
       </c>
-      <c r="D2" s="3">
-        <v>-2.4980018054066019E-14</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="D2">
+        <v>-1.110223024625157E-14</v>
+      </c>
+      <c r="E2">
         <v>67</v>
       </c>
-      <c r="F2" s="3">
-        <v>30.0959</v>
-      </c>
-      <c r="G2" s="3">
-        <v>46.301400000000001</v>
-      </c>
-      <c r="H2" s="3">
-        <v>37.801350000000014</v>
-      </c>
-      <c r="I2" s="3">
-        <v>37.801350000000014</v>
+      <c r="F2">
+        <v>50.4375</v>
+      </c>
+      <c r="G2">
+        <v>50.4375</v>
+      </c>
+      <c r="H2">
+        <v>25.562500000000011</v>
+      </c>
+      <c r="I2">
+        <v>25.5625</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3">
+        <v>5.5511151231257827E-15</v>
+      </c>
+      <c r="C3">
         <v>50</v>
       </c>
-      <c r="D3" s="3">
-        <v>-2.4980018054066019E-14</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3">
+        <v>-1.110223024625157E-14</v>
+      </c>
+      <c r="E3">
         <v>67</v>
       </c>
-      <c r="F3" s="3">
-        <v>30.0959</v>
-      </c>
-      <c r="G3" s="3">
-        <v>46.301400000000001</v>
-      </c>
-      <c r="H3" s="3">
-        <v>37.801350000000014</v>
-      </c>
-      <c r="I3" s="3">
-        <v>37.801350000000014</v>
+      <c r="F3">
+        <v>50.4375</v>
+      </c>
+      <c r="G3">
+        <v>50.4375</v>
+      </c>
+      <c r="H3">
+        <v>25.562500000000011</v>
+      </c>
+      <c r="I3">
+        <v>25.5625</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4">
+        <v>5.5511151231257827E-15</v>
+      </c>
+      <c r="C4">
         <v>50</v>
       </c>
-      <c r="D4" s="3">
-        <v>-2.4980018054066019E-14</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4">
+        <v>-1.110223024625157E-14</v>
+      </c>
+      <c r="E4">
         <v>67</v>
       </c>
-      <c r="F4" s="3">
-        <v>30.0959</v>
-      </c>
-      <c r="G4" s="3">
-        <v>46.301400000000001</v>
-      </c>
-      <c r="H4" s="3">
-        <v>37.801350000000014</v>
-      </c>
-      <c r="I4" s="3">
-        <v>37.801350000000014</v>
+      <c r="F4">
+        <v>50.4375</v>
+      </c>
+      <c r="G4">
+        <v>50.4375</v>
+      </c>
+      <c r="H4">
+        <v>25.562500000000011</v>
+      </c>
+      <c r="I4">
+        <v>25.5625</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>50</v>
       </c>
-      <c r="D5" s="3">
-        <v>-5.5511151231257827E-15</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5">
+        <v>5.5511151231257827E-15</v>
+      </c>
+      <c r="E5">
         <v>87.000000000000014</v>
       </c>
-      <c r="F5" s="3">
-        <v>30.0959</v>
-      </c>
-      <c r="G5" s="3">
-        <v>46.301400000000001</v>
-      </c>
-      <c r="H5" s="3">
-        <v>27.801349999999999</v>
-      </c>
-      <c r="I5" s="3">
-        <v>27.801349999999999</v>
+      <c r="F5">
+        <v>50.4375</v>
+      </c>
+      <c r="G5">
+        <v>50.4375</v>
+      </c>
+      <c r="H5">
+        <v>15.562500000000011</v>
+      </c>
+      <c r="I5">
+        <v>15.562500000000011</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>50</v>
       </c>
-      <c r="D6" s="3">
-        <v>-5.5511151231257827E-15</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6">
+        <v>5.5511151231257827E-15</v>
+      </c>
+      <c r="E6">
         <v>87.000000000000014</v>
       </c>
-      <c r="F6" s="3">
-        <v>30.0959</v>
-      </c>
-      <c r="G6" s="3">
-        <v>46.301400000000001</v>
-      </c>
-      <c r="H6" s="3">
-        <v>27.801349999999999</v>
-      </c>
-      <c r="I6" s="3">
-        <v>27.801349999999999</v>
+      <c r="F6">
+        <v>50.4375</v>
+      </c>
+      <c r="G6">
+        <v>50.4375</v>
+      </c>
+      <c r="H6">
+        <v>15.562500000000011</v>
+      </c>
+      <c r="I6">
+        <v>15.562500000000011</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>50</v>
       </c>
-      <c r="D7" s="3">
-        <v>-5.5511151231257827E-15</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="D7">
+        <v>5.5511151231257827E-15</v>
+      </c>
+      <c r="E7">
         <v>87.000000000000014</v>
       </c>
-      <c r="F7" s="3">
-        <v>30.0959</v>
-      </c>
-      <c r="G7" s="3">
-        <v>46.301400000000001</v>
-      </c>
-      <c r="H7" s="3">
-        <v>27.801349999999999</v>
-      </c>
-      <c r="I7" s="3">
-        <v>27.801349999999999</v>
+      <c r="F7">
+        <v>50.4375</v>
+      </c>
+      <c r="G7">
+        <v>50.4375</v>
+      </c>
+      <c r="H7">
+        <v>15.562500000000011</v>
+      </c>
+      <c r="I7">
+        <v>15.562500000000011</v>
       </c>
     </row>
   </sheetData>
@@ -3011,9 +1840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3051,7 +1878,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -3063,7 +1890,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G2">
         <v>60</v>
@@ -3080,7 +1907,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -3092,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G3">
         <v>60</v>
@@ -3109,7 +1936,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3121,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G4">
         <v>60</v>
@@ -3138,7 +1965,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -3150,7 +1977,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G5">
         <v>60</v>
@@ -3167,7 +1994,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -3179,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G6">
         <v>60</v>
@@ -3196,7 +2023,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -3208,7 +2035,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G7">
         <v>60</v>
@@ -3222,7 +2049,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3230,9 +2056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3343,9 +2167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3383,10 +2205,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>67.25</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3395,16 +2217,16 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>30.0959</v>
+        <v>50.4375</v>
       </c>
       <c r="G2">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="H2">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="I2">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3412,10 +2234,10 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>67.25</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -3424,16 +2246,16 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>30.0959</v>
+        <v>50.4375</v>
       </c>
       <c r="G3">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="H3">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="I3">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3441,10 +2263,10 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>67.25</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3453,16 +2275,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>30.0959</v>
+        <v>50.4375</v>
       </c>
       <c r="G4">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="H4">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="I4">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3470,10 +2292,10 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>67.25</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3482,16 +2304,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>30.0959</v>
+        <v>50.4375</v>
       </c>
       <c r="G5">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="H5">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="I5">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3499,10 +2321,10 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>67.25</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3511,16 +2333,16 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>30.0959</v>
+        <v>50.4375</v>
       </c>
       <c r="G6">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="H6">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="I6">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -3528,10 +2350,10 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>67.25</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -3540,16 +2362,16 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>30.0959</v>
+        <v>50.4375</v>
       </c>
       <c r="G7">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="H7">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
       <c r="I7">
-        <v>46.301400000000001</v>
+        <v>50.4375</v>
       </c>
     </row>
   </sheetData>
@@ -3599,7 +2421,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -3611,16 +2433,16 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3628,7 +2450,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -3640,16 +2462,16 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3657,7 +2479,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3669,16 +2491,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3686,7 +2508,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -3698,16 +2520,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3715,7 +2537,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -3727,16 +2549,16 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -3744,7 +2566,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -3756,16 +2578,16 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3777,7 +2599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3815,7 +2637,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3844,7 +2666,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3873,7 +2695,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3902,7 +2724,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3931,7 +2753,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3960,7 +2782,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -4043,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -4072,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -4101,7 +2923,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -4130,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -4159,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -4188,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -4209,9 +3031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4245,177 +3065,177 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G2" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H2" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I2" s="5">
-        <v>3.847583643122674</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G3" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H3" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I3" s="5">
-        <v>3.847583643122674</v>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G4" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H4" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I4" s="5">
-        <v>3.847583643122674</v>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G5" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H5" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I5" s="5">
-        <v>3.847583643122674</v>
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="I5">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G6" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H6" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I6" s="5">
-        <v>3.847583643122674</v>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G7" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H7" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I7" s="5">
-        <v>3.847583643122674</v>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -4427,9 +3247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4466,174 +3284,174 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>5.8321739726027424</v>
-      </c>
-      <c r="G2" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="H2" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="I2" s="5">
-        <v>8.9725753424657562</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>5.8321739726027424</v>
-      </c>
-      <c r="G3" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="H3" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="I3" s="5">
-        <v>8.9725753424657562</v>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>5.8321739726027424</v>
-      </c>
-      <c r="G4" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="H4" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="I4" s="5">
-        <v>8.9725753424657562</v>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>5.8321739726027424</v>
-      </c>
-      <c r="G5" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="H5" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="I5" s="5">
-        <v>8.9725753424657562</v>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>5.8321739726027424</v>
-      </c>
-      <c r="G6" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="H6" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="I6" s="5">
-        <v>8.9725753424657562</v>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>5.8321739726027424</v>
-      </c>
-      <c r="G7" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="H7" s="5">
-        <v>8.9725753424657562</v>
-      </c>
-      <c r="I7" s="5">
-        <v>8.9725753424657562</v>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4645,9 +3463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4684,174 +3500,174 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>8.5000499999999874</v>
-      </c>
-      <c r="I2" s="6">
-        <v>8.5000499999999874</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>24.874999999999989</v>
+      </c>
+      <c r="I2">
+        <v>24.875</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>8.5000499999999874</v>
-      </c>
-      <c r="I3" s="6">
-        <v>8.5000499999999874</v>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>24.874999999999989</v>
+      </c>
+      <c r="I3">
+        <v>24.875</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>8.5000499999999874</v>
-      </c>
-      <c r="I4" s="6">
-        <v>8.5000499999999874</v>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>24.874999999999989</v>
+      </c>
+      <c r="I4">
+        <v>24.875</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>18.500049999999991</v>
-      </c>
-      <c r="I5" s="6">
-        <v>18.500049999999991</v>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>34.874999999999993</v>
+      </c>
+      <c r="I5">
+        <v>34.874999999999993</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>18.500049999999991</v>
-      </c>
-      <c r="I6" s="6">
-        <v>18.500049999999991</v>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>34.874999999999993</v>
+      </c>
+      <c r="I6">
+        <v>34.874999999999993</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>18.500049999999991</v>
-      </c>
-      <c r="I7" s="6">
-        <v>18.500049999999991</v>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>34.874999999999993</v>
+      </c>
+      <c r="I7">
+        <v>34.874999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -4913,16 +3729,16 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G2">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H2">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I2">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -4942,16 +3758,16 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G3">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H3">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I3">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -4971,16 +3787,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G4">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H4">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I4">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -5000,16 +3816,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G5">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H5">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I5">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -5029,16 +3845,16 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G6">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H6">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I6">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -5058,16 +3874,16 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G7">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H7">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I7">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -5129,16 +3945,16 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -5158,16 +3974,16 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -5187,16 +4003,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -5216,16 +4032,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -5245,16 +4061,16 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -5274,16 +4090,16 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>0.14954292237442929</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5351,10 +4167,10 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.1835808420479724</v>
+        <v>0.49318463444857469</v>
       </c>
       <c r="I2">
-        <v>0.1835808420479724</v>
+        <v>0.49318463444857502</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -5380,10 +4196,10 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.1835808420479724</v>
+        <v>0.49318463444857469</v>
       </c>
       <c r="I3">
-        <v>0.1835808420479724</v>
+        <v>0.49318463444857502</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -5409,10 +4225,10 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0.1835808420479724</v>
+        <v>0.49318463444857469</v>
       </c>
       <c r="I4">
-        <v>0.1835808420479724</v>
+        <v>0.49318463444857502</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -5438,10 +4254,10 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0.3995570328327005</v>
+        <v>0.69144981412639395</v>
       </c>
       <c r="I5">
-        <v>0.3995570328327005</v>
+        <v>0.69144981412639395</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -5467,10 +4283,10 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0.3995570328327005</v>
+        <v>0.69144981412639395</v>
       </c>
       <c r="I6">
-        <v>0.3995570328327005</v>
+        <v>0.69144981412639395</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -5496,10 +4312,10 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0.3995570328327005</v>
+        <v>0.69144981412639395</v>
       </c>
       <c r="I7">
-        <v>0.3995570328327005</v>
+        <v>0.69144981412639395</v>
       </c>
     </row>
   </sheetData>
@@ -5534,10 +4350,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>76.397300000000001</v>
+        <v>100.875</v>
       </c>
       <c r="C2">
-        <v>125.6027</v>
+        <v>101.125</v>
       </c>
       <c r="D2">
         <v>67</v>
@@ -5548,10 +4364,10 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>76.397300000000001</v>
+        <v>100.875</v>
       </c>
       <c r="C3">
-        <v>125.6027</v>
+        <v>101.125</v>
       </c>
       <c r="D3">
         <v>67</v>
@@ -5562,10 +4378,10 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>76.397300000000001</v>
+        <v>100.875</v>
       </c>
       <c r="C4">
-        <v>125.6027</v>
+        <v>101.125</v>
       </c>
       <c r="D4">
         <v>67</v>
@@ -5576,10 +4392,10 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>76.397300000000001</v>
+        <v>100.875</v>
       </c>
       <c r="C5">
-        <v>105.6027</v>
+        <v>81.125000000000028</v>
       </c>
       <c r="D5">
         <v>87.000000000000014</v>
@@ -5590,10 +4406,10 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>76.397300000000001</v>
+        <v>100.875</v>
       </c>
       <c r="C6">
-        <v>105.6027</v>
+        <v>81.125000000000028</v>
       </c>
       <c r="D6">
         <v>87.000000000000014</v>
@@ -5604,10 +4420,10 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>76.397300000000001</v>
+        <v>100.875</v>
       </c>
       <c r="C7">
-        <v>105.6027</v>
+        <v>81.125000000000028</v>
       </c>
       <c r="D7">
         <v>87.000000000000014</v>
@@ -5756,10 +4572,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>126.3973</v>
+        <v>100.875</v>
       </c>
       <c r="C2">
-        <v>142.6028</v>
+        <v>168.125</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5770,10 +4586,10 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>126.3973</v>
+        <v>100.875</v>
       </c>
       <c r="C3">
-        <v>142.6028</v>
+        <v>168.125</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -5784,10 +4600,10 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>126.3973</v>
+        <v>100.875</v>
       </c>
       <c r="C4">
-        <v>142.6028</v>
+        <v>168.125</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -5798,10 +4614,10 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>126.3973</v>
+        <v>100.875</v>
       </c>
       <c r="C5">
-        <v>142.6028</v>
+        <v>168.125</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -5812,10 +4628,10 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>126.3973</v>
+        <v>100.875</v>
       </c>
       <c r="C6">
-        <v>142.6028</v>
+        <v>168.125</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -5826,10 +4642,10 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>126.3973</v>
+        <v>100.875</v>
       </c>
       <c r="C7">
-        <v>142.6028</v>
+        <v>168.125</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -5978,7 +4794,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -5992,7 +4808,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -6006,7 +4822,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -6020,7 +4836,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -6034,7 +4850,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -6048,7 +4864,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -6089,10 +4905,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>6.3485130111524128</v>
+        <v>30</v>
       </c>
       <c r="C2">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6103,10 +4919,10 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>6.3485130111524128</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -6117,10 +4933,10 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>6.3485130111524128</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -6131,10 +4947,10 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>6.3485130111524128</v>
+        <v>30</v>
       </c>
       <c r="C5">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -6145,10 +4961,10 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>6.3485130111524128</v>
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6159,10 +4975,10 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>6.3485130111524128</v>
+        <v>30</v>
       </c>
       <c r="C7">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6200,10 +5016,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>14.8047493150685</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>17.945150684931509</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6214,10 +5030,10 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>14.8047493150685</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>17.945150684931509</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -6228,10 +5044,10 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>14.8047493150685</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>17.945150684931509</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -6242,10 +5058,10 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>14.8047493150685</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>17.945150684931509</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -6256,10 +5072,10 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>14.8047493150685</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>17.945150684931509</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6270,10 +5086,10 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>14.8047493150685</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>17.945150684931509</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6282,265 +5098,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100206C8747921DEB47908282AF5FC82B21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd288e11850d22ee40981664a927e65e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dce361f-7b53-4909-8b0d-30e42626cdc9" xmlns:ns3="3610aed6-0335-46d2-b190-87c476b048cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8a8939e80faa41470004db56e4a3333" ns2:_="" ns3:_="">
-    <xsd:import namespace="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
-    <xsd:import namespace="3610aed6-0335-46d2-b190-87c476b048cc"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6dce361f-7b53-4909-8b0d-30e42626cdc9" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="11" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="87865813-b24e-4515-aac3-72cd3b0aa1df" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="19" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="20" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:description="" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3610aed6-0335-46d2-b190-87c476b048cc" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{afb7282a-b4e1-44aa-9a85-3d59d972ca27}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="3610aed6-0335-46d2-b190-87c476b048cc">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72171B7B-BC50-41AB-AF8B-08DE7C7165EB}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D557DC51-3A44-490A-84F5-B34A74C5F208}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F2679F2-3871-45B4-B542-5C39ED9265E6}"/>
 </file>
</xml_diff>

<commit_message>
added Ireland testcase, updated model to be based on ireland.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="11_7D95A7C73E3670CDB74D5D1D2BF767C2935C3038" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F66021E-6C8E-4606-87A0-DFB900B467C1}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_A559E053343FCEED4E86D6259C507F0EAE3E5418" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2725045D-9671-4259-8159-39672611AEF6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -162,9 +162,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,25 +214,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -252,1157 +234,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Market</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="ltUpDiag">
-              <a:fgClr>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>PG_MARKET!$B$1:$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>G1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>G2.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>G2.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>G3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>W1.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>W1.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>W2.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>W2.2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>PG_MARKET!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7D27-450A-88D2-4FD2608D2BFF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Curtailed</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="openDmnd">
-              <a:fgClr>
-                <a:schemeClr val="accent6"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>PG_MARKET!$B$1:$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>G1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>G2.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>G2.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>G3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>W1.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>W1.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>W2.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>W2.2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>PG_SECURE!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30.0959</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>46.301400000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>46.301400000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>46.301400000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7D27-450A-88D2-4FD2608D2BFF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Constrained</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>PG_MARKET!$B$1:$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>G1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>G2.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>G2.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>G3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>W1.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>W1.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>W2.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>W2.2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>pG!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2.4980018054066019E-14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30.0959</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>46.301400000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>37.801350000000014</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>37.801350000000014</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7D27-450A-88D2-4FD2608D2BFF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="2102019391"/>
-        <c:axId val="2102019871"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2102019391"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2102019871"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2102019871"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="800" b="0"/>
-                  <a:t>Generator</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="800" b="0" baseline="0"/>
-                  <a:t> Power (MW)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB" sz="800" b="0"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2102019391"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr>
-          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4248D362-0D2D-D2EC-B0B3-96547B818B7E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1694,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1753,230 +584,230 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
         <v>269.00000000000011</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2">
         <v>269.00000000000011</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2">
         <v>117</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2">
         <v>240</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2">
         <v>21</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2">
         <v>152</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2">
         <v>66.999999999999972</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2">
         <v>49.999899999999997</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2">
         <v>17.249999999999989</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2">
         <v>32.749900000000018</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2">
         <v>17.000099999999971</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>269.00000000000011</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3">
         <v>269.00000000000011</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3">
         <v>117</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3">
         <v>240</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3">
         <v>21</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3">
         <v>152</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3">
         <v>66.999999999999972</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3">
         <v>49.999899999999997</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3">
         <v>17.249999999999989</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3">
         <v>32.749900000000018</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3">
         <v>17.000099999999971</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>269.00000000000011</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>269.00000000000011</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>117</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>240</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4">
         <v>21</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4">
         <v>152</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4">
         <v>66.999999999999972</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4">
         <v>49.999899999999997</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4">
         <v>17.249999999999989</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4">
         <v>32.749900000000018</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
         <v>17.000099999999971</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>269.00000000000011</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5">
         <v>269.00000000000011</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>137</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>240</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5">
         <v>21</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5">
         <v>132</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5">
         <v>86.999999999999986</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5">
         <v>49.999899999999997</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5">
         <v>17.249999999999989</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5">
         <v>32.749900000000018</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5">
         <v>37.000099999999989</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>269.00000000000011</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>269.00000000000011</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>137</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>240</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
         <v>21</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6">
         <v>132</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6">
         <v>86.999999999999986</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6">
         <v>49.999899999999997</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6">
         <v>17.249999999999989</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6">
         <v>32.749900000000018</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6">
         <v>37.000099999999989</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>269.00000000000011</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>269.00000000000011</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>137</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>240</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
         <v>21</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7">
         <v>132</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7">
         <v>86.999999999999986</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7">
         <v>49.999899999999997</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7">
         <v>17.249999999999989</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7">
         <v>32.749900000000018</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7">
         <v>37.000099999999989</v>
       </c>
     </row>
@@ -2793,9 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2829,176 +1658,176 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>50</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2">
         <v>-2.4980018054066019E-14</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>67</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2">
         <v>30.0959</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2">
         <v>46.301400000000001</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2">
         <v>37.801350000000014</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2">
         <v>37.801350000000014</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>50</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>-2.4980018054066019E-14</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>67</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>30.0959</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <v>46.301400000000001</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3">
         <v>37.801350000000014</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3">
         <v>37.801350000000014</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>50</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>-2.4980018054066019E-14</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>67</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
         <v>30.0959</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <v>46.301400000000001</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4">
         <v>37.801350000000014</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4">
         <v>37.801350000000014</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>50</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>-5.5511151231257827E-15</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>87.000000000000014</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>30.0959</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>46.301400000000001</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5">
         <v>27.801349999999999</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5">
         <v>27.801349999999999</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>50</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>-5.5511151231257827E-15</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>87.000000000000014</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>30.0959</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>46.301400000000001</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6">
         <v>27.801349999999999</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6">
         <v>27.801349999999999</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>50</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>-5.5511151231257827E-15</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>87.000000000000014</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>30.0959</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <v>46.301400000000001</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7">
         <v>27.801349999999999</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7">
         <v>27.801349999999999</v>
       </c>
     </row>
@@ -3011,9 +1840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3222,7 +2049,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3230,9 +2056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3343,9 +2167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4209,9 +3031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4245,177 +3065,177 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G2" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H2" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I2" s="5">
-        <v>3.847583643122674</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>9.75</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G3" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H3" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I3" s="5">
-        <v>3.847583643122674</v>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>9.75</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G4" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H4" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I4" s="5">
-        <v>3.847583643122674</v>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>9.75</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G5" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H5" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I5" s="5">
-        <v>3.847583643122674</v>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>9.75</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="I5">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G6" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H6" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I6" s="5">
-        <v>3.847583643122674</v>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>9.75</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>2.500929368029738</v>
-      </c>
-      <c r="G7" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="H7" s="5">
-        <v>3.847583643122674</v>
-      </c>
-      <c r="I7" s="5">
-        <v>3.847583643122674</v>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>9.75</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -4427,9 +3247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4466,28 +3284,28 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>5.8321739726027424</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2">
         <v>8.9725753424657562</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2">
         <v>8.9725753424657562</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2">
         <v>8.9725753424657562</v>
       </c>
     </row>
@@ -4495,28 +3313,28 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>5.8321739726027424</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3">
         <v>8.9725753424657562</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3">
         <v>8.9725753424657562</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3">
         <v>8.9725753424657562</v>
       </c>
     </row>
@@ -4524,28 +3342,28 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>5.8321739726027424</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4">
         <v>8.9725753424657562</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4">
         <v>8.9725753424657562</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4">
         <v>8.9725753424657562</v>
       </c>
     </row>
@@ -4553,28 +3371,28 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>5.8321739726027424</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5">
         <v>8.9725753424657562</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5">
         <v>8.9725753424657562</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5">
         <v>8.9725753424657562</v>
       </c>
     </row>
@@ -4582,28 +3400,28 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>5.8321739726027424</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6">
         <v>8.9725753424657562</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6">
         <v>8.9725753424657562</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6">
         <v>8.9725753424657562</v>
       </c>
     </row>
@@ -4611,28 +3429,28 @@
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>5.8321739726027424</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7">
         <v>8.9725753424657562</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7">
         <v>8.9725753424657562</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7">
         <v>8.9725753424657562</v>
       </c>
     </row>
@@ -4645,9 +3463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4684,28 +3500,28 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>8.5000499999999874</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2">
         <v>8.5000499999999874</v>
       </c>
     </row>
@@ -4713,28 +3529,28 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>8.5000499999999874</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3">
         <v>8.5000499999999874</v>
       </c>
     </row>
@@ -4742,28 +3558,28 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>8.5000499999999874</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4">
         <v>8.5000499999999874</v>
       </c>
     </row>
@@ -4771,28 +3587,28 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>18.500049999999991</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5">
         <v>18.500049999999991</v>
       </c>
     </row>
@@ -4800,28 +3616,28 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>18.500049999999991</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6">
         <v>18.500049999999991</v>
       </c>
     </row>
@@ -4829,28 +3645,28 @@
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>18.500049999999991</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7">
         <v>18.500049999999991</v>
       </c>
     </row>
@@ -4913,16 +3729,16 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G2">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H2">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I2">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -4942,16 +3758,16 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G3">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H3">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I3">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -4971,16 +3787,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G4">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H4">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I4">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -5000,16 +3816,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G5">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H5">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I5">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -5029,16 +3845,16 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G6">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H6">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I6">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -5058,16 +3874,16 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G7">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="H7">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I7">
-        <v>6.4126394052044566E-2</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -6089,10 +4905,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>6.3485130111524128</v>
+        <v>24.75</v>
       </c>
       <c r="C2">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6103,10 +4919,10 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>6.3485130111524128</v>
+        <v>24.75</v>
       </c>
       <c r="C3">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -6117,10 +4933,10 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>6.3485130111524128</v>
+        <v>24.75</v>
       </c>
       <c r="C4">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -6131,10 +4947,10 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>6.3485130111524128</v>
+        <v>24.75</v>
       </c>
       <c r="C5">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -6145,10 +4961,10 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>6.3485130111524128</v>
+        <v>24.75</v>
       </c>
       <c r="C6">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6159,10 +4975,10 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>6.3485130111524128</v>
+        <v>24.75</v>
       </c>
       <c r="C7">
-        <v>7.695167286245348</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6514,15 +5330,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
@@ -6533,14 +5340,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72171B7B-BC50-41AB-AF8B-08DE7C7165EB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B220FB4-04C0-4B75-83E7-4D8D28289FFB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D557DC51-3A44-490A-84F5-B34A74C5F208}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA516FDF-892D-4A8A-B9C2-C9DD44DD9EBB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F2679F2-3871-45B4-B542-5C39ED9265E6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EF0619-FB91-4643-AF98-17479B3376A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>